<commit_message>
Include Known Issues for each profile in an IG - align formatting
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/practitionerrole-withpractitionerident-1.xlsx
+++ b/output/AdvanceCareRecords/practitionerrole-withpractitionerident-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="376">
   <si>
     <t>Path</t>
   </si>
@@ -153,7 +153,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-prarol-01:The practitioner reference shall at least have a reference or an identifier {practitioner.reference.exists() or practitioner.identifier.exists()}</t>
   </si>
   <si>
     <t>PRD (as one example)</t>
@@ -882,10 +882,6 @@
   </si>
   <si>
     <t>Practitioner that is able to provide the defined services for the organation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-dh-prarol-01:The practitioner shall at least have a reference or an identifier {reference.exists() or identifier.exists()}
-</t>
   </si>
   <si>
     <t>.player</t>
@@ -7837,13 +7833,13 @@
         <v>40</v>
       </c>
       <c r="AI58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK58" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="AJ58" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
@@ -7854,7 +7850,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7877,13 +7873,13 @@
         <v>52</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>278</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>279</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7934,7 +7930,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -7952,7 +7948,7 @@
         <v>40</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>40</v>
@@ -7963,7 +7959,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7989,16 +7985,16 @@
         <v>142</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>284</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>285</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>40</v>
@@ -8023,14 +8019,14 @@
         <v>40</v>
       </c>
       <c r="W60" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="X60" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="X60" t="s" s="2">
+      <c r="Y60" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>288</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>40</v>
       </c>
@@ -8047,7 +8043,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8062,10 +8058,10 @@
         <v>40</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AK60" t="s" s="2">
         <v>289</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>290</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>268</v>
@@ -8076,7 +8072,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8185,7 +8181,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8296,7 +8292,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8368,7 +8364,7 @@
         <v>40</v>
       </c>
       <c r="AA63" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB63" s="2"/>
       <c r="AC63" t="s" s="2">
@@ -8407,10 +8403,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C64" t="s" s="2">
         <v>40</v>
@@ -8435,10 +8431,10 @@
         <v>155</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M64" t="s" s="2">
         <v>158</v>
@@ -8472,10 +8468,10 @@
         <v>136</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Z64" t="s" s="2">
         <v>40</v>
@@ -8522,10 +8518,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C65" t="s" s="2">
         <v>40</v>
@@ -8550,10 +8546,10 @@
         <v>155</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M65" t="s" s="2">
         <v>158</v>
@@ -8587,10 +8583,10 @@
         <v>136</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>40</v>
@@ -8637,7 +8633,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8750,7 +8746,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8776,10 +8772,10 @@
         <v>142</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>303</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>304</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8806,11 +8802,11 @@
         <v>40</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="X67" s="2"/>
       <c r="Y67" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>40</v>
@@ -8828,7 +8824,7 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -8843,13 +8839,13 @@
         <v>40</v>
       </c>
       <c r="AJ67" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AK67" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="AK67" t="s" s="2">
+      <c r="AL67" t="s" s="2">
         <v>307</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>308</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>40</v>
@@ -8857,7 +8853,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8880,13 +8876,13 @@
         <v>52</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8937,7 +8933,7 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
@@ -8955,18 +8951,18 @@
         <v>40</v>
       </c>
       <c r="AK68" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AL68" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="AL68" t="s" s="2">
+      <c r="AM68" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>315</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8989,13 +8985,13 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="K69" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="K69" t="s" s="2">
+      <c r="L69" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -9046,7 +9042,7 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -9061,10 +9057,10 @@
         <v>40</v>
       </c>
       <c r="AJ69" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="AK69" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
@@ -9075,7 +9071,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9098,17 +9094,17 @@
         <v>52</v>
       </c>
       <c r="J70" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="K70" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="K70" t="s" s="2">
+      <c r="L70" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>40</v>
@@ -9157,7 +9153,7 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -9175,7 +9171,7 @@
         <v>40</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>40</v>
@@ -9186,7 +9182,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9209,16 +9205,16 @@
         <v>40</v>
       </c>
       <c r="J71" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="K71" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="K71" t="s" s="2">
+      <c r="L71" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
@@ -9268,7 +9264,7 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9280,13 +9276,13 @@
         <v>40</v>
       </c>
       <c r="AI71" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AJ71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK71" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>40</v>
@@ -9297,7 +9293,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9406,7 +9402,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9517,11 +9513,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9546,7 +9542,7 @@
         <v>103</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M74" t="s" s="2">
         <v>100</v>
@@ -9599,7 +9595,7 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9628,7 +9624,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9654,10 +9650,10 @@
         <v>70</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>343</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -9687,11 +9683,11 @@
         <v>136</v>
       </c>
       <c r="X75" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="Y75" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="Y75" t="s" s="2">
-        <v>345</v>
-      </c>
       <c r="Z75" t="s" s="2">
         <v>40</v>
       </c>
@@ -9708,7 +9704,7 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -9726,7 +9722,7 @@
         <v>40</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
@@ -9737,7 +9733,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9763,10 +9759,10 @@
         <v>253</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9817,7 +9813,7 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -9835,7 +9831,7 @@
         <v>40</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
@@ -9846,7 +9842,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9869,16 +9865,16 @@
         <v>40</v>
       </c>
       <c r="J77" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="K77" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="K77" t="s" s="2">
+      <c r="L77" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>352</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>353</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9928,7 +9924,7 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -9946,7 +9942,7 @@
         <v>40</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
@@ -9957,7 +9953,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9980,16 +9976,16 @@
         <v>40</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="L78" t="s" s="2">
-        <v>356</v>
-      </c>
       <c r="M78" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
@@ -10039,7 +10035,7 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -10057,7 +10053,7 @@
         <v>40</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>40</v>
@@ -10068,7 +10064,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10091,13 +10087,13 @@
         <v>40</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K79" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="L79" t="s" s="2">
         <v>358</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>359</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -10148,7 +10144,7 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -10160,13 +10156,13 @@
         <v>40</v>
       </c>
       <c r="AI79" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AJ79" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK79" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="AJ79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>40</v>
@@ -10177,7 +10173,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10286,7 +10282,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10397,11 +10393,11 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -10426,7 +10422,7 @@
         <v>103</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M82" t="s" s="2">
         <v>100</v>
@@ -10479,7 +10475,7 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10508,7 +10504,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10534,10 +10530,10 @@
         <v>121</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -10588,7 +10584,7 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>51</v>
@@ -10617,7 +10613,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10643,10 +10639,10 @@
         <v>192</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="L84" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="L84" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -10697,7 +10693,7 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
@@ -10715,7 +10711,7 @@
         <v>40</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>40</v>
@@ -10726,7 +10722,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10752,10 +10748,10 @@
         <v>121</v>
       </c>
       <c r="K85" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="L85" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="L85" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -10806,7 +10802,7 @@
         <v>40</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
@@ -10824,7 +10820,7 @@
         <v>40</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>40</v>
@@ -10835,7 +10831,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10858,17 +10854,17 @@
         <v>40</v>
       </c>
       <c r="J86" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="K86" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="K86" t="s" s="2">
+      <c r="L86" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="L86" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>40</v>
@@ -10917,7 +10913,7 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>

</xml_diff>